<commit_message>
Feature: new functions, download excel report and more complete report
</commit_message>
<xml_diff>
--- a/chats/ventas.xlsx
+++ b/chats/ventas.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FD2EF0-9EED-4FD5-93A3-DCA884D42038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Chats" state="visible" r:id="rId4"/>
+    <sheet name="Chats" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="87">
   <si>
     <t>Fecha</t>
   </si>
@@ -28,156 +29,266 @@
     <t>Medio de pago</t>
   </si>
   <si>
-    <t>05-07-23 08:10</t>
-  </si>
-  <si>
-    <t>bombón</t>
-  </si>
-  <si>
-    <t xml:space="preserve">daviplata
-caramelo </t>
-  </si>
-  <si>
-    <t>05-07-23 08:11</t>
-  </si>
-  <si>
-    <t>caramelo</t>
+    <t>08-07-23 10:38</t>
+  </si>
+  <si>
+    <t>Sobre</t>
+  </si>
+  <si>
+    <t>efectivo</t>
+  </si>
+  <si>
+    <t>08-07-23 08:09</t>
+  </si>
+  <si>
+    <t>Peluche vaca</t>
+  </si>
+  <si>
+    <t>Bolsa seda</t>
+  </si>
+  <si>
+    <t>Burbuja jet</t>
+  </si>
+  <si>
+    <t>08-07-23 08:10</t>
+  </si>
+  <si>
+    <t>Cinta pequeña</t>
+  </si>
+  <si>
+    <t>Kuromi</t>
+  </si>
+  <si>
+    <t>Ancheta</t>
+  </si>
+  <si>
+    <t>Rosa</t>
+  </si>
+  <si>
+    <t>Pocillo</t>
+  </si>
+  <si>
+    <t>Empaque</t>
+  </si>
+  <si>
+    <t>Reloj</t>
+  </si>
+  <si>
+    <t>Pin</t>
+  </si>
+  <si>
+    <t>08-07-23 08:11</t>
+  </si>
+  <si>
+    <t>Pikachu</t>
+  </si>
+  <si>
+    <t>Tarjeta</t>
+  </si>
+  <si>
+    <t>Caja</t>
   </si>
   <si>
     <t>nequi</t>
   </si>
   <si>
-    <t>luigi</t>
-  </si>
-  <si>
-    <t>efectivo</t>
-  </si>
-  <si>
-    <t>bolsa de seda</t>
-  </si>
-  <si>
-    <t>cinta</t>
-  </si>
-  <si>
-    <t>05-07-23 08:12</t>
-  </si>
-  <si>
-    <t>05-07-23 09:57</t>
-  </si>
-  <si>
-    <t>dulces</t>
-  </si>
-  <si>
-    <t>05-07-23 11:15</t>
-  </si>
-  <si>
-    <t>azúcar</t>
-  </si>
-  <si>
-    <t>05-07-23 11:16</t>
-  </si>
-  <si>
-    <t>quien</t>
-  </si>
-  <si>
-    <t>de azúcar</t>
-  </si>
-  <si>
-    <t>quiero</t>
-  </si>
-  <si>
-    <t>06-07-23 10:13</t>
-  </si>
-  <si>
-    <t>06-07-23 10:16</t>
-  </si>
-  <si>
-    <t>06-07-23 10:17</t>
-  </si>
-  <si>
-    <t>06-07-23 10:24</t>
-  </si>
-  <si>
-    <t>06-07-23 11:18</t>
-  </si>
-  <si>
-    <t>dulce</t>
-  </si>
-  <si>
-    <t>06-07-23 11:33</t>
-  </si>
-  <si>
-    <t>colbon</t>
-  </si>
-  <si>
-    <t>06-07-23 11:48</t>
-  </si>
-  <si>
-    <t>peluche</t>
-  </si>
-  <si>
-    <t>ancheta</t>
-  </si>
-  <si>
-    <t>06-07-23 11:49</t>
-  </si>
-  <si>
-    <t>cuaderno</t>
+    <t>08-07-23 08:12</t>
+  </si>
+  <si>
+    <t>Burbujas</t>
+  </si>
+  <si>
+    <t>Chocolatinas jet</t>
+  </si>
+  <si>
+    <t>Gol</t>
+  </si>
+  <si>
+    <t>Choco Break</t>
+  </si>
+  <si>
+    <t>Globo helio marcado</t>
+  </si>
+  <si>
+    <t>09-07-23 11:06</t>
+  </si>
+  <si>
+    <t>Impresión</t>
+  </si>
+  <si>
+    <t>Almendras pequeñas</t>
+  </si>
+  <si>
+    <t>09-07-23 11:26</t>
+  </si>
+  <si>
+    <t>Cariñosito</t>
+  </si>
+  <si>
+    <t>09-07-23 12:27</t>
+  </si>
+  <si>
+    <t>Adhesivo Tarjeta</t>
+  </si>
+  <si>
+    <t>09-07-23 01:00</t>
+  </si>
+  <si>
+    <t>Globo helio grande</t>
+  </si>
+  <si>
+    <t>Globo helio pequeño</t>
+  </si>
+  <si>
+    <t>Palo Globo</t>
+  </si>
+  <si>
+    <t>09-07-23 01:01</t>
+  </si>
+  <si>
+    <t>Pocillo ancheta</t>
+  </si>
+  <si>
+    <t>09-07-23 01:11</t>
+  </si>
+  <si>
+    <t>09-07-23 01:12</t>
+  </si>
+  <si>
+    <t>Bolsa de regalo</t>
+  </si>
+  <si>
+    <t>Trululu chocolores</t>
+  </si>
+  <si>
+    <t>09-07-23 02:17</t>
+  </si>
+  <si>
+    <t>Mantel fiesta</t>
+  </si>
+  <si>
+    <t>Vela volcán</t>
+  </si>
+  <si>
+    <t>Vela whiskey</t>
+  </si>
+  <si>
+    <t>Papel brillante</t>
+  </si>
+  <si>
+    <t>09-07-23 03:36</t>
+  </si>
+  <si>
+    <t>Bolsa regalo</t>
+  </si>
+  <si>
+    <t>09-07-23 03:37</t>
+  </si>
+  <si>
+    <t>Globo mediano</t>
+  </si>
+  <si>
+    <t>09-07-23 04:20</t>
+  </si>
+  <si>
+    <t>Vaso cervecero</t>
+  </si>
+  <si>
+    <t>09-07-23 04:46</t>
+  </si>
+  <si>
+    <t>09-07-23 05:02</t>
+  </si>
+  <si>
+    <t>Hello Kitty</t>
+  </si>
+  <si>
+    <t>09-07-23 05:03</t>
+  </si>
+  <si>
+    <t>Burbujas jet</t>
+  </si>
+  <si>
+    <t>Quipitos</t>
+  </si>
+  <si>
+    <t>09-07-23 05:04</t>
+  </si>
+  <si>
+    <t>09-07-23 07:32</t>
+  </si>
+  <si>
+    <t>09-07-23 07:59</t>
+  </si>
+  <si>
+    <t>Pepa Pig</t>
+  </si>
+  <si>
+    <t>09-07-23 08:00</t>
+  </si>
+  <si>
+    <t>09-07-23 08:28</t>
+  </si>
+  <si>
+    <t>Copias</t>
+  </si>
+  <si>
+    <t>Arreglo de flores</t>
+  </si>
+  <si>
+    <t>10-07-23 12:49</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Oso eco</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bolsas regalo</t>
+  </si>
+  <si>
+    <t>10-07-23 03:40</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ancheta</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> collar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bolsa regalo</t>
   </si>
   <si>
     <t>daviplata</t>
   </si>
   <si>
-    <t>06-07-23 07:22</t>
-  </si>
-  <si>
-    <t>perrito</t>
-  </si>
-  <si>
-    <t>06-07-23 07:23</t>
-  </si>
-  <si>
-    <t>carro</t>
-  </si>
-  <si>
-    <t>06-07-23 09:58</t>
-  </si>
-  <si>
-    <t>jet jumbo</t>
-  </si>
-  <si>
-    <t>06-07-23 10:03</t>
-  </si>
-  <si>
-    <t>06-07-23 10:48</t>
-  </si>
-  <si>
-    <t>burbuja</t>
-  </si>
-  <si>
-    <t>06-07-23 10:55</t>
-  </si>
-  <si>
-    <t>07-07-23 12:00</t>
-  </si>
-  <si>
-    <t>07-07-23 12:03</t>
-  </si>
-  <si>
-    <t>07-07-23 12:05</t>
+    <t>10-07-23 04:10</t>
+  </si>
+  <si>
+    <t>10-07-23 04:48</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bombas helio</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> velas palitos</t>
+  </si>
+  <si>
+    <t>10-07-23 04:55</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> luigi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -540,17 +651,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" defaultColWidth="9.140625"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5703125" customWidth="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1"/>
   </cols>
@@ -577,7 +688,7 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>5000</v>
+        <v>1500</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -588,13 +699,13 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -602,13 +713,13 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C4">
-        <v>70000</v>
+        <v>1500</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -616,13 +727,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C5">
-        <v>1500000</v>
+        <v>56000</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -630,353 +741,941 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C6">
-        <v>200000</v>
+        <v>2500</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C7">
-        <v>300</v>
+        <v>900</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C8">
-        <v>52000</v>
+        <v>800</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C9">
-        <v>5000</v>
+        <v>38000</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C10">
-        <v>5000</v>
+        <v>20200</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C11">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
       </c>
       <c r="C12">
-        <v>5000</v>
+        <v>8000</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C13">
-        <v>5000</v>
+        <v>3800</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C14">
-        <v>5000</v>
+        <v>25000</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C15">
-        <v>5000</v>
+        <v>1500</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C16">
-        <v>5000</v>
+        <v>2500</v>
       </c>
       <c r="D16" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C17">
-        <v>5000</v>
+        <v>15000</v>
       </c>
       <c r="D17" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C18">
-        <v>70000</v>
+        <v>1500</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="C19">
-        <v>40000</v>
+        <v>1500</v>
       </c>
       <c r="D19" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C20">
-        <v>15000</v>
+        <v>300</v>
       </c>
       <c r="D20" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="C21">
-        <v>15000</v>
+        <v>6000</v>
       </c>
       <c r="D21" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="C22">
-        <v>20000</v>
+        <v>8000</v>
       </c>
       <c r="D22" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="C23">
-        <v>3500</v>
+        <v>1500</v>
       </c>
       <c r="D23" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C24">
-        <v>3500</v>
+        <v>1800</v>
       </c>
       <c r="D24" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="C25">
-        <v>3500</v>
+        <v>1600</v>
       </c>
       <c r="D25" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C26">
-        <v>34000</v>
+        <v>1600</v>
       </c>
       <c r="D26" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C27">
-        <v>50000</v>
+        <v>600</v>
       </c>
       <c r="D27" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="C28">
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="D28" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="B29" t="s">
         <v>32</v>
       </c>
       <c r="C29">
-        <v>50000</v>
+        <v>2300</v>
       </c>
       <c r="D29" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
         <v>33</v>
       </c>
       <c r="C30">
-        <v>40000</v>
+        <v>3300</v>
       </c>
       <c r="D30" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31">
+        <v>87000</v>
+      </c>
+      <c r="D31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32">
+        <v>2500</v>
+      </c>
+      <c r="D32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33">
+        <v>300</v>
+      </c>
+      <c r="D33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34">
+        <v>7000</v>
+      </c>
+      <c r="D34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35">
+        <v>3000</v>
+      </c>
+      <c r="D35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36">
+        <v>400</v>
+      </c>
+      <c r="D36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37">
+        <v>2500</v>
+      </c>
+      <c r="D37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38">
+        <v>15500</v>
+      </c>
+      <c r="D38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39">
+        <v>1500</v>
+      </c>
+      <c r="D39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40">
+        <v>1800</v>
+      </c>
+      <c r="D40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41">
+        <v>1400</v>
+      </c>
+      <c r="D41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42">
+        <v>8000</v>
+      </c>
+      <c r="D42" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43">
+        <v>2000</v>
+      </c>
+      <c r="D43" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>48</v>
+      </c>
+      <c r="B44" t="s">
+        <v>51</v>
+      </c>
+      <c r="C44">
+        <v>3000</v>
+      </c>
+      <c r="D44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45">
+        <v>4800</v>
+      </c>
+      <c r="D45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46" t="s">
+        <v>54</v>
+      </c>
+      <c r="C46">
+        <v>4600</v>
+      </c>
+      <c r="D46" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47">
+        <v>5000</v>
+      </c>
+      <c r="D47" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48" t="s">
+        <v>58</v>
+      </c>
+      <c r="C48">
+        <v>16000</v>
+      </c>
+      <c r="D48" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>59</v>
+      </c>
+      <c r="B49" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49">
+        <v>20400</v>
+      </c>
+      <c r="D49" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>60</v>
+      </c>
+      <c r="B50" t="s">
+        <v>61</v>
+      </c>
+      <c r="C50">
+        <v>23000</v>
+      </c>
+      <c r="D50" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51" t="s">
+        <v>47</v>
+      </c>
+      <c r="C51">
+        <v>1400</v>
+      </c>
+      <c r="D51" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>62</v>
+      </c>
+      <c r="B52" t="s">
+        <v>63</v>
+      </c>
+      <c r="C52">
+        <v>1800</v>
+      </c>
+      <c r="D52" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>62</v>
+      </c>
+      <c r="B53" t="s">
+        <v>28</v>
+      </c>
+      <c r="C53">
+        <v>800</v>
+      </c>
+      <c r="D53" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>62</v>
+      </c>
+      <c r="B54" t="s">
+        <v>64</v>
+      </c>
+      <c r="C54">
+        <v>700</v>
+      </c>
+      <c r="D54" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>65</v>
+      </c>
+      <c r="B55" t="s">
+        <v>17</v>
+      </c>
+      <c r="C55">
+        <v>1500</v>
+      </c>
+      <c r="D55" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>66</v>
+      </c>
+      <c r="B56" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56">
+        <v>1500</v>
+      </c>
+      <c r="D56" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57" t="s">
+        <v>18</v>
+      </c>
+      <c r="C57">
+        <v>21000</v>
+      </c>
+      <c r="D57" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>67</v>
+      </c>
+      <c r="B58" t="s">
+        <v>68</v>
+      </c>
+      <c r="C58">
+        <v>12000</v>
+      </c>
+      <c r="D58" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>67</v>
+      </c>
+      <c r="B59" t="s">
+        <v>68</v>
+      </c>
+      <c r="C59">
+        <v>12000</v>
+      </c>
+      <c r="D59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>69</v>
+      </c>
+      <c r="B60" t="s">
+        <v>17</v>
+      </c>
+      <c r="C60">
+        <v>2500</v>
+      </c>
+      <c r="D60" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>69</v>
+      </c>
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61">
+        <v>700</v>
+      </c>
+      <c r="D61" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>70</v>
+      </c>
+      <c r="B62" t="s">
+        <v>71</v>
+      </c>
+      <c r="C62">
+        <v>1200</v>
+      </c>
+      <c r="D62" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>70</v>
+      </c>
+      <c r="B63" t="s">
+        <v>72</v>
+      </c>
+      <c r="C63">
+        <v>4400</v>
+      </c>
+      <c r="D63" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>73</v>
+      </c>
+      <c r="B64" t="s">
+        <v>74</v>
+      </c>
+      <c r="C64">
+        <v>14000</v>
+      </c>
+      <c r="D64" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>73</v>
+      </c>
+      <c r="B65" t="s">
+        <v>75</v>
+      </c>
+      <c r="C65">
+        <v>2500</v>
+      </c>
+      <c r="D65" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>76</v>
+      </c>
+      <c r="B66" t="s">
+        <v>77</v>
+      </c>
+      <c r="C66">
+        <v>55000</v>
+      </c>
+      <c r="D66" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>76</v>
+      </c>
+      <c r="B67" t="s">
+        <v>78</v>
+      </c>
+      <c r="C67">
+        <v>15000</v>
+      </c>
+      <c r="D67" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>76</v>
+      </c>
+      <c r="B68" t="s">
+        <v>79</v>
+      </c>
+      <c r="C68">
+        <v>1800</v>
+      </c>
+      <c r="D68" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>81</v>
+      </c>
+      <c r="B69" t="s">
+        <v>77</v>
+      </c>
+      <c r="C69">
+        <v>23000</v>
+      </c>
+      <c r="D69" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>82</v>
+      </c>
+      <c r="B70" t="s">
+        <v>83</v>
+      </c>
+      <c r="C70">
+        <v>7500</v>
+      </c>
+      <c r="D70" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>82</v>
+      </c>
+      <c r="B71" t="s">
+        <v>84</v>
+      </c>
+      <c r="C71">
+        <v>4000</v>
+      </c>
+      <c r="D71" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>85</v>
+      </c>
+      <c r="B72" t="s">
+        <v>86</v>
+      </c>
+      <c r="C72">
+        <v>30000</v>
+      </c>
+      <c r="D72" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>